<commit_message>
Trying to get comparable figures for Chart
</commit_message>
<xml_diff>
--- a/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
+++ b/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Algorithm #1</t>
   </si>
@@ -108,6 +109,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Operations</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> per N</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -145,12 +176,139 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>183600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>675021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3717990</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15437221</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$1:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18787</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>315636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>624294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1320288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2892157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5994378</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11931650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm #3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -160,10 +318,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$A$31</c:f>
-              <c:strCache>
-                <c:ptCount val="31"/>
+            <c:numRef>
+              <c:f>Sheet1!$I$1:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>250</c:v>
                 </c:pt>
@@ -177,150 +336,78 @@
                   <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Algorithm #1</c:v>
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>200000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>400000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Algorithm #2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>400000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Algorithm #2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>400000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>800000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1600000</c:v>
-                </c:pt>
-                <c:pt idx="28">
                   <c:v>3200000</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="12">
                   <c:v>6400000</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>Algorithm #3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$31</c:f>
+              <c:f>Sheet1!$J$1:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>183600</c:v>
+                  <c:v>1246</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>675021</c:v>
+                  <c:v>2496</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3717990</c:v>
+                  <c:v>4996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15437221</c:v>
+                  <c:v>9996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>249996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>288630</c:v>
+                  <c:v>499996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>616095</c:v>
+                  <c:v>999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1314800</c:v>
+                  <c:v>1999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2829350</c:v>
+                  <c:v>3999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5789254</c:v>
+                  <c:v>7999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11885052</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>287571</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>658426</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1313056</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2595811</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5980548</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11951098</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>499996</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>999996</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3999996</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7999996</c:v>
-                </c:pt>
-                <c:pt idx="28">
                   <c:v>15999996</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="12">
                   <c:v>31999996</c:v>
                 </c:pt>
               </c:numCache>
@@ -337,11 +424,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="410743464"/>
-        <c:axId val="410748952"/>
+        <c:axId val="412812104"/>
+        <c:axId val="412812496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="410743464"/>
+        <c:axId val="412812104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,15 +471,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410748952"/>
+        <c:crossAx val="412812496"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="410748952"/>
+        <c:axId val="412812496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410743464"/>
+        <c:crossAx val="412812104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -455,6 +543,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -484,11 +604,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1048,25 +1163,28 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8663836" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1079,7 +1197,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1346,239 +1464,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" activeCellId="2" sqref="D1:D4 G1:G10 J1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="2" max="2" width="1.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>250</v>
       </c>
       <c r="B1">
         <v>183600</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>250</v>
+      </c>
+      <c r="D1">
+        <v>183600</v>
+      </c>
+      <c r="F1">
+        <v>250</v>
+      </c>
+      <c r="G1">
+        <v>1741</v>
+      </c>
+      <c r="I1">
+        <v>250</v>
+      </c>
+      <c r="J1">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500</v>
       </c>
       <c r="B2">
         <v>675021</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>675021</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>3899</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+      <c r="J2">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
       <c r="B3">
         <v>3717990</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>3717990</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>9397</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
       <c r="B4">
         <v>15437221</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>15437221</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+      <c r="G4">
+        <v>18787</v>
+      </c>
+      <c r="I4">
+        <v>2000</v>
+      </c>
+      <c r="J4">
+        <v>9996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="F5">
+        <v>25000</v>
+      </c>
+      <c r="G5">
+        <v>315636</v>
+      </c>
+      <c r="I5">
+        <v>25000</v>
+      </c>
+      <c r="J5">
+        <v>124996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>50000</v>
+      </c>
+      <c r="G6">
+        <v>624294</v>
+      </c>
+      <c r="I6">
+        <v>50000</v>
+      </c>
+      <c r="J6">
+        <v>249996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25000</v>
       </c>
       <c r="B7">
         <v>288630</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>100000</v>
+      </c>
+      <c r="G7">
+        <v>1320288</v>
+      </c>
+      <c r="I7">
+        <v>100000</v>
+      </c>
+      <c r="J7">
+        <v>499996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50000</v>
       </c>
       <c r="B8">
         <v>616095</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>200000</v>
+      </c>
+      <c r="G8">
+        <v>2892157</v>
+      </c>
+      <c r="I8">
+        <v>200000</v>
+      </c>
+      <c r="J8">
+        <v>999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100000</v>
       </c>
       <c r="B9">
         <v>1314800</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>400000</v>
+      </c>
+      <c r="G9">
+        <v>5994378</v>
+      </c>
+      <c r="I9">
+        <v>400000</v>
+      </c>
+      <c r="J9">
+        <v>1999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>200000</v>
       </c>
       <c r="B10">
         <v>2829350</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>800000</v>
+      </c>
+      <c r="G10">
+        <v>11931650</v>
+      </c>
+      <c r="I10">
+        <v>800000</v>
+      </c>
+      <c r="J10">
+        <v>3999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>400000</v>
       </c>
       <c r="B11">
         <v>5789254</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="I11">
+        <v>1600000</v>
+      </c>
+      <c r="J11">
+        <v>7999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>800000</v>
       </c>
       <c r="B12">
         <v>11885052</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>3200000</v>
+      </c>
+      <c r="J12">
+        <v>15999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>6400000</v>
+      </c>
+      <c r="J13">
+        <v>31999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="I14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="F15">
         <v>25000</v>
       </c>
-      <c r="B16">
+      <c r="G15">
         <v>287571</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>50000</v>
+      </c>
+      <c r="G16">
+        <v>658426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>100000</v>
+      </c>
+      <c r="B17">
+        <v>499996</v>
+      </c>
+      <c r="F17">
+        <v>100000</v>
+      </c>
+      <c r="G17">
+        <v>1313056</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>200000</v>
+      </c>
+      <c r="B18">
+        <v>999996</v>
+      </c>
+      <c r="F18">
+        <v>200000</v>
+      </c>
+      <c r="G18">
+        <v>2595811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>400000</v>
+      </c>
+      <c r="B19">
+        <v>1999996</v>
+      </c>
+      <c r="F19">
+        <v>400000</v>
+      </c>
+      <c r="G19">
+        <v>5980548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>800000</v>
+      </c>
+      <c r="B20">
+        <v>3999996</v>
+      </c>
+      <c r="F20">
+        <v>800000</v>
+      </c>
+      <c r="G20">
+        <v>11951098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1600000</v>
+      </c>
+      <c r="B21">
+        <v>7999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3200000</v>
+      </c>
+      <c r="B22">
+        <v>15999996</v>
+      </c>
+      <c r="F22">
+        <v>25000</v>
+      </c>
+      <c r="G22">
+        <v>288630</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6400000</v>
+      </c>
+      <c r="B23">
+        <v>31999996</v>
+      </c>
+      <c r="F23">
         <v>50000</v>
       </c>
-      <c r="B17">
-        <v>658426</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="G23">
+        <v>616095</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="F24">
         <v>100000</v>
       </c>
-      <c r="B18">
-        <v>1313056</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="G24">
+        <v>1314800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25">
         <v>200000</v>
       </c>
-      <c r="B19">
-        <v>2595811</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="G25">
+        <v>2829350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26">
         <v>400000</v>
       </c>
-      <c r="B20">
-        <v>5980548</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="G26">
+        <v>5789254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27">
         <v>800000</v>
       </c>
-      <c r="B21">
-        <v>11951098</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>100000</v>
-      </c>
-      <c r="B24">
-        <v>499996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>200000</v>
-      </c>
-      <c r="B25">
-        <v>999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>400000</v>
-      </c>
-      <c r="B26">
-        <v>1999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>800000</v>
-      </c>
-      <c r="B27">
-        <v>3999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1600000</v>
-      </c>
-      <c r="B28">
-        <v>7999996</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3200000</v>
-      </c>
-      <c r="B29">
-        <v>15999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>6400000</v>
-      </c>
-      <c r="B30">
-        <v>31999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2"/>
+      <c r="G27">
+        <v>11885052</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF000000"/>
+          <x14:colorNegative rgb="FF0070C0"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF0070C0"/>
+          <x14:colorFirst rgb="FF0070C0"/>
+          <x14:colorLast rgb="FF0070C0"/>
+          <x14:colorHigh rgb="FF0070C0"/>
+          <x14:colorLow rgb="FF0070C0"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!D1:D1</xm:f>
+              <xm:sqref>C1</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D2:D2</xm:f>
+              <xm:sqref>C2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D3:D3</xm:f>
+              <xm:sqref>C3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D4:D4</xm:f>
+              <xm:sqref>C4</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF000000"/>
           <x14:colorNegative rgb="FF0070C0"/>

</xml_diff>

<commit_message>
Completed comparison of running times
</commit_message>
<xml_diff>
--- a/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
+++ b/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
@@ -180,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$5</c:f>
+              <c:f>Sheet1!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -203,10 +203,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$4</c:f>
+              <c:f>Sheet1!$D$1:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>183600</c:v>
                 </c:pt>
@@ -218,6 +218,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15437221</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127400626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -229,7 +232,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$11</c:f>
+              <c:f>Sheet1!$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -252,39 +255,48 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$1:$G$10</c:f>
+              <c:f>Sheet1!$G$1:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1741</c:v>
+                  <c:v>1884</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3899</c:v>
+                  <c:v>3635</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9397</c:v>
+                  <c:v>8203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18787</c:v>
+                  <c:v>18034</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>315636</c:v>
+                  <c:v>302033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>624294</c:v>
+                  <c:v>602483</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1320288</c:v>
+                  <c:v>1269942</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2892157</c:v>
+                  <c:v>2851193</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5994378</c:v>
+                  <c:v>5615718</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11931650</c:v>
+                  <c:v>12020323</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24964641</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53696043</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>110758696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" activeCellId="2" sqref="D1:D4 G1:G10 J1:J13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1505,7 @@
         <v>250</v>
       </c>
       <c r="G1">
-        <v>1741</v>
+        <v>1884</v>
       </c>
       <c r="I1">
         <v>250</v>
@@ -1519,7 +1531,7 @@
         <v>500</v>
       </c>
       <c r="G2">
-        <v>3899</v>
+        <v>3635</v>
       </c>
       <c r="I2">
         <v>500</v>
@@ -1545,7 +1557,7 @@
         <v>1000</v>
       </c>
       <c r="G3">
-        <v>9397</v>
+        <v>8203</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -1571,7 +1583,7 @@
         <v>2000</v>
       </c>
       <c r="G4">
-        <v>18787</v>
+        <v>18034</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1585,15 +1597,17 @@
         <v>0</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="C5">
+        <v>25000</v>
+      </c>
+      <c r="D5">
+        <v>127400626</v>
+      </c>
       <c r="F5">
         <v>25000</v>
       </c>
       <c r="G5">
-        <v>315636</v>
+        <v>302033</v>
       </c>
       <c r="I5">
         <v>25000</v>
@@ -1603,11 +1617,15 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="F6">
         <v>50000</v>
       </c>
       <c r="G6">
-        <v>624294</v>
+        <v>602483</v>
       </c>
       <c r="I6">
         <v>50000</v>
@@ -1627,7 +1645,7 @@
         <v>100000</v>
       </c>
       <c r="G7">
-        <v>1320288</v>
+        <v>1269942</v>
       </c>
       <c r="I7">
         <v>100000</v>
@@ -1647,7 +1665,7 @@
         <v>200000</v>
       </c>
       <c r="G8">
-        <v>2892157</v>
+        <v>2851193</v>
       </c>
       <c r="I8">
         <v>200000</v>
@@ -1667,7 +1685,7 @@
         <v>400000</v>
       </c>
       <c r="G9">
-        <v>5994378</v>
+        <v>5615718</v>
       </c>
       <c r="I9">
         <v>400000</v>
@@ -1687,7 +1705,7 @@
         <v>800000</v>
       </c>
       <c r="G10">
-        <v>11931650</v>
+        <v>12020323</v>
       </c>
       <c r="I10">
         <v>800000</v>
@@ -1703,10 +1721,12 @@
       <c r="B11">
         <v>5789254</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="F11">
+        <v>1600000</v>
+      </c>
+      <c r="G11">
+        <v>24964641</v>
+      </c>
       <c r="I11">
         <v>1600000</v>
       </c>
@@ -1721,6 +1741,12 @@
       <c r="B12">
         <v>11885052</v>
       </c>
+      <c r="F12">
+        <v>3200000</v>
+      </c>
+      <c r="G12">
+        <v>53696043</v>
+      </c>
       <c r="I12">
         <v>3200000</v>
       </c>
@@ -1729,6 +1755,12 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>6400000</v>
+      </c>
+      <c r="G13">
+        <v>110758696</v>
+      </c>
       <c r="I13">
         <v>6400000</v>
       </c>
@@ -1741,8 +1773,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2"/>
       <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1751,20 +1785,6 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="F15">
-        <v>25000</v>
-      </c>
-      <c r="G15">
-        <v>287571</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16">
-        <v>50000</v>
-      </c>
-      <c r="G16">
-        <v>658426</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1774,10 +1794,10 @@
         <v>499996</v>
       </c>
       <c r="F17">
-        <v>100000</v>
+        <v>250</v>
       </c>
       <c r="G17">
-        <v>1313056</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1788,10 +1808,10 @@
         <v>999996</v>
       </c>
       <c r="F18">
-        <v>200000</v>
+        <v>500</v>
       </c>
       <c r="G18">
-        <v>2595811</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1802,10 +1822,10 @@
         <v>1999996</v>
       </c>
       <c r="F19">
-        <v>400000</v>
+        <v>1000</v>
       </c>
       <c r="G19">
-        <v>5980548</v>
+        <v>9397</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1816,10 +1836,10 @@
         <v>3999996</v>
       </c>
       <c r="F20">
-        <v>800000</v>
+        <v>2000</v>
       </c>
       <c r="G20">
-        <v>11951098</v>
+        <v>18787</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1829,6 +1849,12 @@
       <c r="B21">
         <v>7999996</v>
       </c>
+      <c r="F21">
+        <v>25000</v>
+      </c>
+      <c r="G21">
+        <v>315636</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1838,10 +1864,10 @@
         <v>15999996</v>
       </c>
       <c r="F22">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="G22">
-        <v>288630</v>
+        <v>624294</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1852,10 +1878,10 @@
         <v>31999996</v>
       </c>
       <c r="F23">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="G23">
-        <v>616095</v>
+        <v>1320288</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,33 +1890,125 @@
       </c>
       <c r="B24" s="2"/>
       <c r="F24">
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="G24">
-        <v>1314800</v>
+        <v>2892157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25">
-        <v>200000</v>
+        <v>400000</v>
       </c>
       <c r="G25">
-        <v>2829350</v>
+        <v>5994378</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F26">
+        <v>800000</v>
+      </c>
+      <c r="G26">
+        <v>11931650</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>25000</v>
+      </c>
+      <c r="G28">
+        <v>287571</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>50000</v>
+      </c>
+      <c r="G29">
+        <v>658426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>100000</v>
+      </c>
+      <c r="G30">
+        <v>1313056</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>200000</v>
+      </c>
+      <c r="G31">
+        <v>2595811</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32">
         <v>400000</v>
       </c>
-      <c r="G26">
+      <c r="G32">
+        <v>5980548</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>800000</v>
+      </c>
+      <c r="G33">
+        <v>11951098</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>25000</v>
+      </c>
+      <c r="G35">
+        <v>288630</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>50000</v>
+      </c>
+      <c r="G36">
+        <v>616095</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>100000</v>
+      </c>
+      <c r="G37">
+        <v>1314800</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>200000</v>
+      </c>
+      <c r="G38">
+        <v>2829350</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>400000</v>
+      </c>
+      <c r="G39">
         <v>5789254</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40">
         <v>800000</v>
       </c>
-      <c r="G27">
+      <c r="G40">
         <v>11885052</v>
       </c>
     </row>
@@ -1900,8 +2018,8 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
tweeking k n^2 and n^3 to get better run time figures
</commit_message>
<xml_diff>
--- a/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
+++ b/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Algorithm #1</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>Algorithm #3</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>n^3</t>
   </si>
 </sst>
 </file>
@@ -115,13 +124,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -129,13 +144,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of Operations</a:t>
+              <a:t>Number of Operations per N</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> per N</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -153,13 +163,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -190,13 +206,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -242,13 +264,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -318,13 +346,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -421,6 +455,230 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>31999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Linear</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$1:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9600000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19200000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>N^2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$1:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2250000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>81000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>n^3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$1:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>421875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3375000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15625000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42875000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91125000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>125000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,11 +694,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="412812104"/>
-        <c:axId val="412812496"/>
+        <c:axId val="110854600"/>
+        <c:axId val="110853032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="412812104"/>
+        <c:axId val="110854600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,9 +712,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -470,9 +728,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -483,7 +740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412812496"/>
+        <c:crossAx val="110853032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -492,7 +749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="412812496"/>
+        <c:axId val="110853032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,9 +759,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -530,9 +787,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -543,7 +799,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412812104"/>
+        <c:crossAx val="110854600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,9 +829,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -592,17 +847,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -660,35 +926,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -696,26 +960,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -724,9 +996,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -745,14 +1016,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -761,45 +1024,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -811,31 +1064,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -853,21 +1104,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -877,20 +1125,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -904,14 +1152,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -925,9 +1173,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -941,12 +1188,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -958,9 +1199,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -975,14 +1216,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -994,14 +1234,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1013,14 +1253,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1029,14 +1268,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1044,7 +1282,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1057,11 +1295,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1069,14 +1317,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1088,12 +1336,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1109,7 +1364,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1118,9 +1372,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1130,7 +1383,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1138,9 +1391,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1151,9 +1404,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1165,12 +1417,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1179,7 +1425,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1190,7 +1436,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8672180" cy="6302006"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1476,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P6:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1734,7 @@
     <col min="2" max="2" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>250</v>
       </c>
@@ -1513,8 +1759,30 @@
       <c r="J1">
         <v>1246</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1">
+        <v>250</v>
+      </c>
+      <c r="M1">
+        <f>L1*M$16</f>
+        <v>1500</v>
+      </c>
+      <c r="N1">
+        <v>10</v>
+      </c>
+      <c r="O1">
+        <f>(L1/10)^2</f>
+        <v>625</v>
+      </c>
+      <c r="P1">
+        <f>(N1*P$16)^2</f>
+        <v>40000</v>
+      </c>
+      <c r="Q1">
+        <f>N1^3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500</v>
       </c>
@@ -1533,14 +1801,40 @@
       <c r="G2">
         <v>3635</v>
       </c>
+      <c r="H2">
+        <f>G2/G1</f>
+        <v>1.9294055201698515</v>
+      </c>
       <c r="I2">
         <v>500</v>
       </c>
       <c r="J2">
         <v>2496</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>500</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M13" si="0">L2*M$16</f>
+        <v>3000</v>
+      </c>
+      <c r="N2">
+        <v>20</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O4" si="1">(L2/10)^2</f>
+        <v>2500</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P13" si="2">(N2*P$16)^2</f>
+        <v>160000</v>
+      </c>
+      <c r="Q2">
+        <f>N2^3</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -1559,14 +1853,40 @@
       <c r="G3">
         <v>8203</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="3">G3/G2</f>
+        <v>2.256671251719395</v>
+      </c>
       <c r="I3">
         <v>1000</v>
       </c>
       <c r="J3">
         <v>4996</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q13" si="4">N3^3</f>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -1585,14 +1905,40 @@
       <c r="G4">
         <v>18034</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>2.1984639765939291</v>
+      </c>
       <c r="I4">
         <v>2000</v>
       </c>
       <c r="J4">
         <v>9996</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>2000</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>12000</v>
+      </c>
+      <c r="N4">
+        <v>75</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>2250000</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="4"/>
+        <v>421875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1615,8 +1961,30 @@
       <c r="J5">
         <v>124996</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>25000</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5">
+        <f>(L5/100)^2</f>
+        <v>62500</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>4000000</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1627,14 +1995,40 @@
       <c r="G6">
         <v>602483</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>1.9947588508540457</v>
+      </c>
       <c r="I6">
         <v>50000</v>
       </c>
       <c r="J6">
         <v>249996</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>50000</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="N6">
+        <v>150</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="5">(L6/100)^2</f>
+        <v>250000</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>9000000</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="4"/>
+        <v>3375000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25000</v>
       </c>
@@ -1647,14 +2041,40 @@
       <c r="G7">
         <v>1269942</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>2.1078470263891265</v>
+      </c>
       <c r="I7">
         <v>100000</v>
       </c>
       <c r="J7">
         <v>499996</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>100000</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="N7">
+        <v>200</v>
+      </c>
+      <c r="O7">
+        <f>(L7/200)^2</f>
+        <v>250000</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>16000000</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="4"/>
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50000</v>
       </c>
@@ -1667,14 +2087,40 @@
       <c r="G8">
         <v>2851193</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>2.2451363920557004</v>
+      </c>
       <c r="I8">
         <v>200000</v>
       </c>
       <c r="J8">
         <v>999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>200000</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>1200000</v>
+      </c>
+      <c r="N8">
+        <v>250</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O12" si="6">(L8/200)^2</f>
+        <v>1000000</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>25000000</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="4"/>
+        <v>15625000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100000</v>
       </c>
@@ -1687,14 +2133,40 @@
       <c r="G9">
         <v>5615718</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>1.9696028995581849</v>
+      </c>
       <c r="I9">
         <v>400000</v>
       </c>
       <c r="J9">
         <v>1999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>400000</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>2400000</v>
+      </c>
+      <c r="N9">
+        <v>300</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>4000000</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>36000000</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>27000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>200000</v>
       </c>
@@ -1707,14 +2179,40 @@
       <c r="G10">
         <v>12020323</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>2.1404783858448733</v>
+      </c>
       <c r="I10">
         <v>800000</v>
       </c>
       <c r="J10">
         <v>3999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>800000</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>4800000</v>
+      </c>
+      <c r="N10">
+        <v>350</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>16000000</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>49000000</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="4"/>
+        <v>42875000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>400000</v>
       </c>
@@ -1727,14 +2225,40 @@
       <c r="G11">
         <v>24964641</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>2.0768693986010192</v>
+      </c>
       <c r="I11">
         <v>1600000</v>
       </c>
       <c r="J11">
         <v>7999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>1600000</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>9600000</v>
+      </c>
+      <c r="N11">
+        <v>400</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>64000000</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>64000000</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="4"/>
+        <v>64000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>800000</v>
       </c>
@@ -1747,28 +2271,76 @@
       <c r="G12">
         <v>53696043</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>2.1508838440737041</v>
+      </c>
       <c r="I12">
         <v>3200000</v>
       </c>
       <c r="J12">
         <v>15999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>3200000</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>19200000</v>
+      </c>
+      <c r="N12">
+        <v>450</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>256000000</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>81000000</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="4"/>
+        <v>91125000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>6400000</v>
       </c>
       <c r="G13">
         <v>110758696</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>2.0626975436532633</v>
+      </c>
       <c r="I13">
         <v>6400000</v>
       </c>
       <c r="J13">
         <v>31999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>6400000</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>38400000</v>
+      </c>
+      <c r="N13">
+        <v>500</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>100000000</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>125000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1781,10 +2353,30 @@
         <v>2</v>
       </c>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="P16">
+        <v>20</v>
+      </c>
+      <c r="Q16">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">

</xml_diff>

<commit_message>
creating a scatter plot for Algorithm #3
</commit_message>
<xml_diff>
--- a/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
+++ b/JamiSchwarzwalder-Assignment1/Runtime of Algorithms.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Algorithm #1" sheetId="3" r:id="rId2"/>
     <sheet name="Algorithm #2" sheetId="5" r:id="rId3"/>
     <sheet name="Algorithm #3" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Algorithm #3 Scatter" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -152,6 +153,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -696,11 +698,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="319825784"/>
-        <c:axId val="319827352"/>
+        <c:axId val="366929600"/>
+        <c:axId val="366924896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319825784"/>
+        <c:axId val="366929600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319827352"/>
+        <c:crossAx val="366924896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319827352"/>
+        <c:axId val="366924896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319825784"/>
+        <c:crossAx val="366929600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -815,6 +817,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -926,7 +929,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1053,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="319824216"/>
-        <c:axId val="319829704"/>
+        <c:axId val="366926856"/>
+        <c:axId val="366927248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319824216"/>
+        <c:axId val="366926856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,7 +1101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319829704"/>
+        <c:crossAx val="366927248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1107,7 +1109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319829704"/>
+        <c:axId val="366927248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,7 +1160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319824216"/>
+        <c:crossAx val="366926856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1172,7 +1174,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1683,11 +1684,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="319830096"/>
-        <c:axId val="319826568"/>
+        <c:axId val="316976432"/>
+        <c:axId val="316979176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319830096"/>
+        <c:axId val="316976432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,7 +1731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319826568"/>
+        <c:crossAx val="316979176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1738,7 +1739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319826568"/>
+        <c:axId val="316979176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319830096"/>
+        <c:crossAx val="316976432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1956,6 +1957,54 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$1:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3200000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$J$1:$J$13</c:f>
@@ -2027,6 +2076,54 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$1:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3200000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$M$1:$M$13</c:f>
@@ -2086,16 +2183,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="321706712"/>
-        <c:axId val="321699264"/>
+        <c:axId val="316980744"/>
+        <c:axId val="316978000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="321706712"/>
+        <c:axId val="316980744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2132,7 +2230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321699264"/>
+        <c:crossAx val="316978000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2140,7 +2238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321699264"/>
+        <c:axId val="316978000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321706712"/>
+        <c:crossAx val="316980744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2235,6 +2333,507 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm #3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$1:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3200000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$1:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>249996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>499996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$1:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3200000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$1:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="373628984"/>
+        <c:axId val="373626240"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="373628984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373626240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="373626240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373628984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2427,6 +3026,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -4452,6 +5091,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4497,7 +5652,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4509,6 +5664,17 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4573,7 +5739,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672180" cy="6302006"/>
+    <xdr:ext cx="8672015" cy="6297873"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4597,6 +5763,33 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8672015" cy="6297873"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -4888,8 +6081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5879,6 +7072,34 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF000000"/>
+          <x14:colorNegative rgb="FF0070C0"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF0070C0"/>
+          <x14:colorFirst rgb="FF0070C0"/>
+          <x14:colorLast rgb="FF0070C0"/>
+          <x14:colorHigh rgb="FF0070C0"/>
+          <x14:colorLow rgb="FF0070C0"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B1:B1</xm:f>
+              <xm:sqref>A1</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B2:B2</xm:f>
+              <xm:sqref>A2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B3:B3</xm:f>
+              <xm:sqref>A3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B4:B4</xm:f>
+              <xm:sqref>A4</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF000000"/>
           <x14:colorNegative rgb="FF0070C0"/>
@@ -5907,34 +7128,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF000000"/>
-          <x14:colorNegative rgb="FF0070C0"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF0070C0"/>
-          <x14:colorFirst rgb="FF0070C0"/>
-          <x14:colorLast rgb="FF0070C0"/>
-          <x14:colorHigh rgb="FF0070C0"/>
-          <x14:colorLow rgb="FF0070C0"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!B1:B1</xm:f>
-              <xm:sqref>A1</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!B2:B2</xm:f>
-              <xm:sqref>A2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!B3:B3</xm:f>
-              <xm:sqref>A3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!B4:B4</xm:f>
-              <xm:sqref>A4</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>